<commit_message>
update to inclue play with DataFrame
</commit_message>
<xml_diff>
--- a/openpyxl/pandas_openpyxl.xlsx
+++ b/openpyxl/pandas_openpyxl.xlsx
@@ -400,16 +400,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.539146714475507</v>
+        <v>-0.5105544497887244</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.309539717376205</v>
+        <v>0.4677058628456969</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.205475318566168</v>
+        <v>-0.4252444871073068</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.5208317984461951</v>
+        <v>-0.1454514859615633</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -417,16 +417,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.329790859656458</v>
+        <v>-0.704984082927168</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.031675525339869</v>
+        <v>1.048539417301345</v>
       </c>
       <c r="D3" t="n">
-        <v>1.766459902502809</v>
+        <v>-0.5115076716610412</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.7602141485801279</v>
+        <v>1.128941192698981</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -434,16 +434,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.820521242472361</v>
+        <v>-0.3077101733269968</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.214325677040326</v>
+        <v>0.7499702733889624</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.16918850878801</v>
+        <v>-0.387488401597478</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5055284178390823</v>
+        <v>-1.066945061397698</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -451,16 +451,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.8533606994847929</v>
+        <v>0.3194398239056268</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4485054250301583</v>
+        <v>-0.5509028080077042</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8144500277114802</v>
+        <v>-0.9913314054426073</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.253869460486545</v>
+        <v>0.9453299126560957</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -468,16 +468,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4188554139285804</v>
+        <v>-0.1336755871392932</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.663659442020967</v>
+        <v>-1.015835298249297</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.7270363947129552</v>
+        <v>-1.294854530248012</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.926994264768813</v>
+        <v>-0.7199519196186355</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -485,16 +485,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.5913335978974572</v>
+        <v>-1.226069064553532</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1090217288846918</v>
+        <v>-0.06946859387738215</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02449489462803962</v>
+        <v>-0.2533835077588892</v>
       </c>
       <c r="E7" t="n">
-        <v>1.963529977209435</v>
+        <v>1.097845061231636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>